<commit_message>
refactor: File Controller change xlsx headers
</commit_message>
<xml_diff>
--- a/backend/uploads/stock.xlsx
+++ b/backend/uploads/stock.xlsx
@@ -13,10 +13,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
-    <t>Sku</t>
-  </si>
-  <si>
-    <t>Stock ids</t>
+    <t>Variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock </t>
   </si>
   <si>
     <t>2244-BLSM-L</t>

</xml_diff>

<commit_message>
refactor: use mongodb aggregation
</commit_message>
<xml_diff>
--- a/backend/uploads/stock.xlsx
+++ b/backend/uploads/stock.xlsx
@@ -28,28 +28,28 @@
     <t>2244-BLSM-M</t>
   </si>
   <si>
+    <t>SLKDRM-CLK-52-L</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>SLKDRM-CLK-52-S</t>
+  </si>
+  <si>
     <t>2244-BLSM-S</t>
   </si>
   <si>
+    <t>SLKDRM-CLK-52-XL</t>
+  </si>
+  <si>
+    <t>SLKDRM-CLK-52-M</t>
+  </si>
+  <si>
     <t>2244-BLSM-XL</t>
   </si>
   <si>
     <t>SLKDRM-CLK-03-XL</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>SLKDRM-CLK-52-L</t>
-  </si>
-  <si>
-    <t>SLKDRM-CLK-52-M</t>
-  </si>
-  <si>
-    <t>SLKDRM-CLK-52-S</t>
-  </si>
-  <si>
-    <t>SLKDRM-CLK-52-XL</t>
   </si>
 </sst>
 </file>
@@ -466,23 +466,23 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -490,7 +490,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -498,7 +498,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -506,7 +506,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -514,7 +514,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>